<commit_message>
uncommented samples in input urls
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,66 +473,872 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.eventbrite.com/e/the-rolling-tones-at-hudak-house-tickets-926567788197</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>The Rolling Tones at Hudak House</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Saturday, August 24</t>
-        </is>
-      </c>
+          <t>https://www.eventbrite.com/e/lovemke-summer-soulstice-celebration-tickets-881130915287?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 5737 Orchard Heights Road Northwest Salem, OR 97304 United States</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Hudak House</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.eventbrite.com/e/club-privata-vip-suite-reservations-tickets-321505992077</t>
+          <t>https://www.eventbrite.com/e/fast-track-to-finer-a-series-of-finer-festivities-tickets-897279596427?aff=ebdssbdestsearch</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Club Privata: VIP Suite Reservations</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Friday, June 28</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>Fast Track to Finer "A Series of Finer Festivities"</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$15 – $100</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 824 Southwest 1st Avenue Portland, OR 97204 United States</t>
+          <t xml:space="preserve"> Downtown Indianapolis, IN United States</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Club Privata</t>
+          <t>Zeta Phi Beta Sorority, Inc. - Indiana State Organization</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>297</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/drag-me-to-pride-tickets-896688769247?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/pan-o-prog-speed-puzzle-contest-tickets-887621298197?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pan-O-Prog Speed Puzzle Contest</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Monday, July 8</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sold Out</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pan-O-Prog</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/28th-annual-hbcuc-family-day-black-excellence-rise-up-tickets-904176334757?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/the-hudson-valley-wine-food-festival-tickets-851067855867?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>The Hudson Valley Wine &amp; Food Festival</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Saturday, September 7</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>From $11.59</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6636 U.S. 9 Rhinebeck, NY 12572 United States</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Hudson Valley Wine &amp; Food Festival</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/oaked-and-smoked-american-whiskey-and-bbq-tickets-753421222157?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Oaked and Smoked ~ American Whiskey and BBQ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Saturday, July 13</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$15 – $55</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9568 South University Boulevard Highlands Ranch, CO 80126 United States</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Highlands Ranch Community Association</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>3.5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/fiesta-de-primavera-tickets-886599973387?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/world-food-bazaar-tickets-872835162467?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>580</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/miche-summer-jam-90s-throwback-party-tickets-902431556077?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>385</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/sunshine-serenity-tickets-909985249377?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>224</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/eggfest-greater-moncton-2024-tickets-897445683197?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/ridge-fest-2024-tickets-876212604487?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/nandis-indian-street-food-festival-part-3-tickets-898280961537?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/cuba-caliente-tickets-903841282607?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cuba Caliente</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Saturday, July 27</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 380 Van Wagners Beach Road Hamilton, ON L8E 3L8 Canada</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Javier Martinez</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/15-minutes-of-fame-tickets-860132548607?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>15 Minutes of FAME!</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sunday, August 25</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 202 Martin Avenue Rosebud, AB T0J 2T0 Canada</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Rosebud Festivals</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/celebration-du-30-juin-congo-independence-day-celebration-tickets-914986076987?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Célébration du 30 juin / Congo Independence Day Celebration</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sunday, June 30</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$0 – $400</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1 Tamarac Crescent Southwest Calgary, AB T3C 3B7 Canada</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>SOS Congo Foundation</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/analyticsweek-virtual-job-fair-career-networking-event-vancouver-tickets-131206974593?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AnalyticsWeek Virtual Job Fair / Career Networking Event #Vancouver</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Friday, July 5</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Virtual Event Only Vancouver, BC Canada</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>AnalyticsWEEK</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>8.4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/fire-and-flow-tickets-918485423627?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Fire And Flow</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Friday, July 12</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9692 Jasper Avenue Edmonton, AB T5H 3V5 Canada</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/atl-vegan-festival-tickets-876563213167?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>3.8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/interstate-wine-fest-island-vibes-2024-tickets-775882073167?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2.3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/19th-annual-art-beer-wine-festival-presented-by-county-national-bank-tickets-767051721347?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>251</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/brick-fan-expo-orlando-a-lego-fan-event-tickets-838317148157?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>1.3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/juneteenth-tickets-885418218727?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/2024-beer-festival-tickets-873395458327?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>3.5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/elgin-micheleros-festival-2024-tickets-894092734437?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>416</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/maines-ultimate-spring-yard-sale-seller-spaces-2024-tickets-852245668737?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>215</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/worcester-food-truck-craft-beer-festival-tickets-660552027897?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2.5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/2024-vail-craft-beer-classic-tickets-790474780347?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>667</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/2024-sc-festival-of-flowers-topiaries-tastings-tunes-tickets-881542847387?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/sippin-in-the-south-wine-festival-tickets-789841616537?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/afro-rose-tickets-869144914837?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Afro Rosé</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Sunday, July 7</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>$35 – $99</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1201 Half Street Southeast Washington, DC 20003 United States</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Afro Rose' Group</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/uhuru-liberation-through-education-and-cultural-creativity-tickets-906837123247?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>526</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/randolph-caribbean-american-heritage-festival-tickets-852001037037?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>1.6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/smoke-vine-festival-2024-the-luv-edition-tickets-843802103807?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Smoke &amp; Vine Festival 2024 - The LUV Edition</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Saturday, July 20</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>$35 – $155</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2401 West Leigh Street Richmond, VA 23220 United States</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Michael Braxton</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>773</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/lakefest-oakland-5th-annual-festival-tickets-900823446177?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/13th-annual-stomp-the-blues-festival-tickets-825743690607?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>161</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/2024-brass-screw-consortium-tickets-782975299197?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>116</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/bushels-barrels-local-food-wine-beer-festival-tickets-873395799347?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>388</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/das-energi-2024-tickets-869280059057?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Das Energi 2024</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>$115 – $350</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12408 W Saltair Dr Magna, UT 84044 United States</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>V2 PRESENTS</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>11.4k</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added thread pool executor
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,97 +473,935 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.eventbrite.com/e/fked-up-fairytales-tickets-929488895307?aff=ebdssbdestsearch</t>
+          <t>https://www.eventbrite.com/e/club-privata-vip-suite-reservations-tickets-321505992077?aff=ebdssbdestsearch</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F**ked Up Fairytales</t>
+          <t>Club Privata: VIP Suite Reservations</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Thursday, August 29</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>$25 – $45</t>
-        </is>
-      </c>
+          <t>Friday, June 28</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 3009 Southeast Chestnut Street Portland, OR 97267 United States</t>
+          <t xml:space="preserve"> 824 Southwest 1st Avenue Portland, OR 97204 United States</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sugar &amp; Whiskey Burlesque Company</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>Club Privata</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.3k</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.eventbrite.com/e/drag-brunch-at-freeland-spirits-tickets-926337328887?aff=ebdssbdestsearch</t>
+          <t>https://www.eventbrite.com/e/king-youngblood-tickets-928028778057?aff=ebdssbdestsearch</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Drag Brunch at Freeland Spirits</t>
+          <t>King Youngblood</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Saturday, July 13</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>$13</t>
-        </is>
-      </c>
+          <t>Saturday, August 17</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2671 Northwest Vaughn Street Portland, OR 97210 United States</t>
+          <t xml:space="preserve"> 216 South Tower Avenue Centralia, WA 98531 United States</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Freeland Spirits</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>The Juicebox</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.eventbrite.com/e/red-white-blue-gala-a-salute-to-our-veterans-tickets-882324966727?aff=ebdssbdestsearch</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Red, White &amp; Blue Gala: A Salute to Our Veterans</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Tuesday, July 16</t>
-        </is>
-      </c>
+          <t>https://www.eventbrite.com/e/fog-holler-rusty-cleavers-tickets-924758747307?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 Cowlitz Way Ridgefield, WA 98642 United States</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clark County Veterans Assistance Center</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/the-builders-and-the-butchers-20-year-anniversary-portland-spirit-show-tickets-750049527327?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>The Builders and the Butchers 20 Year Anniversary Portland Spirit Show!!</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Wednesday, October 30</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1010 Southwest Naito Parkway Portland, OR 97204 United States</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>The Builders and the Butchers</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/new-constellations-squirm-happy-hour-music-video-release-party-variety-show-tickets-921070605977?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>New Constellations &amp; Squirm - Happy Hour, Music Video Release Party, &amp; Variety Show</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Thursday, July 25</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$20</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1120 Southeast Madison Street Portland, OR 97214 United States</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/barefoot-fusion-tickets-783186310337?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Barefoot Fusion</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Friday, June 28</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$0 – $15</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6305 Southeast Foster Road Portland, OR 97206 United States</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Portland Blues &amp; Jazz Dance Society</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>162</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/the-umbrellas-love-in-hell-shop-regulars-tickets-872772565237?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>The Umbrellas + Love in Hell + Shop Regulars</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Thursday, June 27</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 727 Southeast Grand Avenue Portland, OR 97214 United States</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Swan Dive Presents</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/romantic-couples-night-butterfly-release-tickets-910166300907?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Romantic Couples Night Butterfly Release</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Friday, July 26</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17005 Northeast Courtney Road Newberg, OR 97132 United States</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Wayward Winds Lavender</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/snow-skate-surf-2024-tickets-785966977387?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>snow skate surf 2024</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Saturday, July 13</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27500 E Timberline Road Government Camp, OR 97028 United States</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>snow skate surf</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/tyrus-live-sept13th-corvallisor-all-new-what-it-is-comedy-tour-tickets-880760808287?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tyrus Live Sept.13th  Corvallis,OR ⭐️ALL NEW “What It Is” Comedy Tour⭐️</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Friday, September 13</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$20 – $300</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4045 Southwest Research Way Corvallis, OR 97333 United States</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Tyrus Live, Inc</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2.2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/country-line-dancing-night-out-tickets-906266666997?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Country Line Dancing Night Out</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Friday, July 12</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 321 Hamilton Road Chehalis, WA 98532 United States</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Gemini Events</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/slumber-party-2024-21-tickets-881681341627?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Slumber Party 2024 (21+)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Saturday, June 29</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$36</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21888 South Fellows Road Estacada, OR 97023 United States</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Last Lesbian Bar Productions</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/stellar-at-soter-a-fundraiser-for-carlton-observatory-tickets-926248623567?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Stellar at Soter - A Fundraiser for Carlton Observatory</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Saturday, September 28</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$100</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10880 Northeast Mineral Springs Road Carlton, OR 97111 United States</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Carlton Observatory at Evergreen</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/class-of-2004-david-douglas-high-school-reunion-tickets-871929162597?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Class of 2004 David Douglas High School Reunion</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sunday, August 11</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$55 – $78</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2126 Southwest Halsey Street Troutdale, OR 97060 United States</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Whitney Bard</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/dd-comedy-presents-tori-piskin-at-the-clinton-street-theater-tickets-922470462987?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>D&amp;D Comedy Presents: Tori Piskin at The Clinton Street Theater</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Thursday, August 1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2522 Southeast Clinton Street Portland, OR 97202 United States</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>D&amp;D Comedy</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>363</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/som3wh3r3-in-n3v3rland-tickets-923183114547?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SOM3WH3R3 IN N3V3RLAND</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Saturday, July 20</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$9 – $99</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3903 North Michigan Avenue Portland, OR 97227 United States</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Som3wh3r3</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/wonka-womp-tickets-928685652787?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Wonka Womp</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Friday, July 5</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 904 Northwest Couch Street Portland, OR 97209 United States</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>FOURTH WORLD PRODUCTIONS</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/american-homeboy-movie-screening-and-lowrider-show-portland-tickets-868018626077?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>"American Homeboy" - Movie Screening and Lowrider Show (Portland)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Saturday, August 17</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12000 Southwest 49th Avenue Portland, OR 97219 United States</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Chela Media</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/lewdicrous-the-burlesque-drag-and-variety-show-of-your-fever-dreams-tickets-926781998907?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>LEWDicrous: the Burlesque, Drag and Variety Show of Your Fever Dreams</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Thursday, July 18</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 727 Southeast Grand Avenue Portland, OR 97214 United States</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Swan Dive Presents</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/grapes-and-grooves-tickets-885698296447?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Grapes and Grooves</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sunday, July 14</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5657 Zena Road Northwest Salem, OR 97304 United States</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Zenith Vineyard</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/club-privata-fishnet-fridays-tickets-905842387967?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Club Privata: Fishnet Fridays</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Friday, August 9</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>$15 – $85</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 824 Southwest 1st Avenue Portland, OR 97204 United States</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Club Privata</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1.3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/roaring-adventures-fire-ice-benefit-gala-3rd-annual-tickets-913178249727?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Roaring Adventures Fire + Ice Benefit Gala, 3rd Annual</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Saturday, November 23</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>$80</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25700 Southwest Petes Mountain Road 25700 SW Petes Mountain Rd, West Linn, OR 97068 West Linn, OR 97068 United States</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Roaring Adventures, Inc.</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/girls-night-out-the-show-at-elks-lodge-1868-white-salmon-wa-tickets-896477527417?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Girls Night Out The Show at Elks Lodge 1868 (White Salmon, WA)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Saturday, September 14</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>From $14.95</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 124  Church Avenue White Salmon, WA 98672 United States</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Girls Night Out the Show</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>36.6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/club-privata-summer-disco-tickets-893373743917?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Club Privata: Summer Disco</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Saturday, July 6</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>$20 – $110</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 824 Southwest 1st Avenue Portland, OR 97204 United States</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Club Privata</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1.3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/handsome-heroes-the-show-in-portland-or-barrel-room-tickets-897558089407?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/bryan-martin-tickets-929192849827?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bryan Martin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Sunday, September 8</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10350 N Vancouver Way Portland, OR 97224 United States</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Ponderosa Lounge and Grill</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>4.2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/reggaetonlandia-portland-21-tickets-925370146017?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>REGGAETONLANDIA, Portland (21+)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Friday, June 28</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 436 NW 6th Ave Portland, OR 97209 United States</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>REGGAETONLANDIA PARTY &amp; EXPERIENCE</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1.6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/portland-new-friends-new-connections-mixer-56-group-tickets-913313955627?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>217</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com/e/dining-with-divas-drag-show-tickets-884285179777?aff=ebdssbdestsearch</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Dining with Divas - Drag Show</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Saturday, June 29</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>$30</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 558 North Market Boulevard Chehalis, WA 98532 United States</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>McFiler's Presents</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>